<commit_message>
More training, changed some rewards
</commit_message>
<xml_diff>
--- a/TrainingModelsDescriptions.xlsx
+++ b/TrainingModelsDescriptions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -51,6 +51,30 @@
   </si>
   <si>
     <t>225k</t>
+  </si>
+  <si>
+    <t>Training3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Training 4</t>
+  </si>
+  <si>
+    <t>23k</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>276k</t>
+  </si>
+  <si>
+    <t>Espersegueixen, cara a cara, s'ataquen a vegades, escut no utilitzat</t>
+  </si>
+  <si>
+    <t>Recompenses per distancia mes petites, canviar recompenses de velocitat I escut</t>
   </si>
 </sst>
 </file>
@@ -384,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,9 +419,10 @@
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="73.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,8 +432,11 @@
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -419,7 +447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -430,19 +458,42 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>